<commit_message>
Excel Extraction  and generated reports by sony
</commit_message>
<xml_diff>
--- a/cypress/fixtures/yearOnYear.xlsx
+++ b/cypress/fixtures/yearOnYear.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -430,22 +430,22 @@
         <v>2025</v>
       </c>
       <c r="B2" t="str">
-        <v>₹ 8,07,191</v>
+        <v>₹ 14,214</v>
       </c>
       <c r="C2" t="str">
-        <v>₹ 69,644</v>
+        <v>₹ 78,999</v>
       </c>
       <c r="D2" t="str">
         <v>₹ 12,500</v>
       </c>
       <c r="E2" t="str">
-        <v>₹ 8,89,335</v>
+        <v>₹ 1,05,713</v>
       </c>
       <c r="F2" t="str">
-        <v>₹ 16,92,809</v>
+        <v>₹ 24,85,786</v>
       </c>
       <c r="G2" t="str">
-        <v>32.29%</v>
+        <v>0.57%</v>
       </c>
     </row>
     <row r="3">
@@ -453,27 +453,464 @@
         <v>2026</v>
       </c>
       <c r="B3" t="str">
-        <v>₹ 16,92,809</v>
+        <v>₹ 45,434</v>
       </c>
       <c r="C3" t="str">
-        <v>₹ 60,861</v>
+        <v>₹ 2,34,205</v>
       </c>
       <c r="D3" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E3" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F3" t="str">
+        <v>₹ 24,40,352</v>
+      </c>
+      <c r="G3" t="str">
+        <v>2.39%</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>2027</v>
+      </c>
+      <c r="B4" t="str">
+        <v>₹ 49,943</v>
+      </c>
+      <c r="C4" t="str">
+        <v>₹ 2,29,696</v>
+      </c>
+      <c r="D4" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E4" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F4" t="str">
+        <v>₹ 23,90,408</v>
+      </c>
+      <c r="G4" t="str">
+        <v>4.38%</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>2028</v>
+      </c>
+      <c r="B5" t="str">
+        <v>₹ 54,900</v>
+      </c>
+      <c r="C5" t="str">
+        <v>₹ 2,24,739</v>
+      </c>
+      <c r="D5" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E5" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F5" t="str">
+        <v>₹ 23,35,508</v>
+      </c>
+      <c r="G5" t="str">
+        <v>6.58%</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>2029</v>
+      </c>
+      <c r="B6" t="str">
+        <v>₹ 60,349</v>
+      </c>
+      <c r="C6" t="str">
+        <v>₹ 2,19,290</v>
+      </c>
+      <c r="D6" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E6" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F6" t="str">
+        <v>₹ 22,75,159</v>
+      </c>
+      <c r="G6" t="str">
+        <v>8.99%</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>2030</v>
+      </c>
+      <c r="B7" t="str">
+        <v>₹ 66,338</v>
+      </c>
+      <c r="C7" t="str">
+        <v>₹ 2,13,301</v>
+      </c>
+      <c r="D7" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E7" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F7" t="str">
+        <v>₹ 22,08,821</v>
+      </c>
+      <c r="G7" t="str">
+        <v>11.65%</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>2031</v>
+      </c>
+      <c r="B8" t="str">
+        <v>₹ 72,922</v>
+      </c>
+      <c r="C8" t="str">
+        <v>₹ 2,06,717</v>
+      </c>
+      <c r="D8" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E8" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F8" t="str">
+        <v>₹ 21,35,899</v>
+      </c>
+      <c r="G8" t="str">
+        <v>14.56%</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>2032</v>
+      </c>
+      <c r="B9" t="str">
+        <v>₹ 80,160</v>
+      </c>
+      <c r="C9" t="str">
+        <v>₹ 1,99,480</v>
+      </c>
+      <c r="D9" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E9" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F9" t="str">
+        <v>₹ 20,55,739</v>
+      </c>
+      <c r="G9" t="str">
+        <v>17.77%</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>2033</v>
+      </c>
+      <c r="B10" t="str">
+        <v>₹ 88,115</v>
+      </c>
+      <c r="C10" t="str">
+        <v>₹ 1,91,524</v>
+      </c>
+      <c r="D10" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E10" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F10" t="str">
+        <v>₹ 19,67,624</v>
+      </c>
+      <c r="G10" t="str">
+        <v>21.3%</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>2034</v>
+      </c>
+      <c r="B11" t="str">
+        <v>₹ 96,861</v>
+      </c>
+      <c r="C11" t="str">
+        <v>₹ 1,82,779</v>
+      </c>
+      <c r="D11" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E11" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F11" t="str">
+        <v>₹ 18,70,763</v>
+      </c>
+      <c r="G11" t="str">
+        <v>25.17%</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>2035</v>
+      </c>
+      <c r="B12" t="str">
+        <v>₹ 1,06,474</v>
+      </c>
+      <c r="C12" t="str">
+        <v>₹ 1,73,166</v>
+      </c>
+      <c r="D12" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E12" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F12" t="str">
+        <v>₹ 17,64,289</v>
+      </c>
+      <c r="G12" t="str">
+        <v>29.43%</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>2036</v>
+      </c>
+      <c r="B13" t="str">
+        <v>₹ 1,17,041</v>
+      </c>
+      <c r="C13" t="str">
+        <v>₹ 1,62,598</v>
+      </c>
+      <c r="D13" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E13" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F13" t="str">
+        <v>₹ 16,47,248</v>
+      </c>
+      <c r="G13" t="str">
+        <v>34.11%</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>2037</v>
+      </c>
+      <c r="B14" t="str">
+        <v>₹ 1,28,657</v>
+      </c>
+      <c r="C14" t="str">
+        <v>₹ 1,50,982</v>
+      </c>
+      <c r="D14" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E14" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F14" t="str">
+        <v>₹ 15,18,591</v>
+      </c>
+      <c r="G14" t="str">
+        <v>39.26%</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>2038</v>
+      </c>
+      <c r="B15" t="str">
+        <v>₹ 1,41,426</v>
+      </c>
+      <c r="C15" t="str">
+        <v>₹ 1,38,213</v>
+      </c>
+      <c r="D15" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E15" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F15" t="str">
+        <v>₹ 13,77,165</v>
+      </c>
+      <c r="G15" t="str">
+        <v>44.91%</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>2039</v>
+      </c>
+      <c r="B16" t="str">
+        <v>₹ 1,55,462</v>
+      </c>
+      <c r="C16" t="str">
+        <v>₹ 1,24,177</v>
+      </c>
+      <c r="D16" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E16" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F16" t="str">
+        <v>₹ 12,21,703</v>
+      </c>
+      <c r="G16" t="str">
+        <v>51.13%</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>2040</v>
+      </c>
+      <c r="B17" t="str">
+        <v>₹ 1,70,891</v>
+      </c>
+      <c r="C17" t="str">
+        <v>₹ 1,08,748</v>
+      </c>
+      <c r="D17" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E17" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F17" t="str">
+        <v>₹ 10,50,812</v>
+      </c>
+      <c r="G17" t="str">
+        <v>57.97%</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>2041</v>
+      </c>
+      <c r="B18" t="str">
+        <v>₹ 1,87,852</v>
+      </c>
+      <c r="C18" t="str">
+        <v>₹ 91,787</v>
+      </c>
+      <c r="D18" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E18" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F18" t="str">
+        <v>₹ 8,62,960</v>
+      </c>
+      <c r="G18" t="str">
+        <v>65.48%</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>2042</v>
+      </c>
+      <c r="B19" t="str">
+        <v>₹ 2,06,496</v>
+      </c>
+      <c r="C19" t="str">
+        <v>₹ 73,144</v>
+      </c>
+      <c r="D19" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E19" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F19" t="str">
+        <v>₹ 6,56,464</v>
+      </c>
+      <c r="G19" t="str">
+        <v>73.74%</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>2043</v>
+      </c>
+      <c r="B20" t="str">
+        <v>₹ 2,26,990</v>
+      </c>
+      <c r="C20" t="str">
+        <v>₹ 52,649</v>
+      </c>
+      <c r="D20" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E20" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F20" t="str">
+        <v>₹ 4,29,474</v>
+      </c>
+      <c r="G20" t="str">
+        <v>82.82%</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>2044</v>
+      </c>
+      <c r="B21" t="str">
+        <v>₹ 2,49,518</v>
+      </c>
+      <c r="C21" t="str">
+        <v>₹ 30,121</v>
+      </c>
+      <c r="D21" t="str">
+        <v>₹ 37,500</v>
+      </c>
+      <c r="E21" t="str">
+        <v>₹ 3,17,139</v>
+      </c>
+      <c r="F21" t="str">
+        <v>₹ 1,79,956</v>
+      </c>
+      <c r="G21" t="str">
+        <v>92.8%</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>2045</v>
+      </c>
+      <c r="B22" t="str">
+        <v>₹ 1,79,956</v>
+      </c>
+      <c r="C22" t="str">
+        <v>₹ 6,470</v>
+      </c>
+      <c r="D22" t="str">
         <v>₹ 25,000</v>
       </c>
-      <c r="E3" t="str">
-        <v>₹ 17,78,670</v>
-      </c>
-      <c r="F3" t="str">
+      <c r="E22" t="str">
+        <v>₹ 2,11,426</v>
+      </c>
+      <c r="F22" t="str">
         <v>₹ 0</v>
       </c>
-      <c r="G3" t="str">
+      <c r="G22" t="str">
         <v>100%</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G22"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Car Loan Calculation committed by Sowmya
</commit_message>
<xml_diff>
--- a/cypress/fixtures/yearOnYear.xlsx
+++ b/cypress/fixtures/yearOnYear.xlsx
@@ -430,22 +430,22 @@
         <v>2025</v>
       </c>
       <c r="B2" t="str">
-        <v>₹ 14,214</v>
+        <v>₹ 15,142</v>
       </c>
       <c r="C2" t="str">
-        <v>₹ 78,999</v>
+        <v>₹ 74,831</v>
       </c>
       <c r="D2" t="str">
         <v>₹ 12,500</v>
       </c>
       <c r="E2" t="str">
-        <v>₹ 1,05,713</v>
+        <v>₹ 1,02,473</v>
       </c>
       <c r="F2" t="str">
-        <v>₹ 24,85,786</v>
+        <v>₹ 24,84,858</v>
       </c>
       <c r="G2" t="str">
-        <v>0.57%</v>
+        <v>0.61%</v>
       </c>
     </row>
     <row r="3">
@@ -453,22 +453,22 @@
         <v>2026</v>
       </c>
       <c r="B3" t="str">
-        <v>₹ 45,434</v>
+        <v>₹ 48,238</v>
       </c>
       <c r="C3" t="str">
-        <v>₹ 2,34,205</v>
+        <v>₹ 2,21,680</v>
       </c>
       <c r="D3" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E3" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F3" t="str">
-        <v>₹ 24,40,352</v>
+        <v>₹ 24,36,620</v>
       </c>
       <c r="G3" t="str">
-        <v>2.39%</v>
+        <v>2.54%</v>
       </c>
     </row>
     <row r="4">
@@ -476,22 +476,22 @@
         <v>2027</v>
       </c>
       <c r="B4" t="str">
-        <v>₹ 49,943</v>
+        <v>₹ 52,763</v>
       </c>
       <c r="C4" t="str">
-        <v>₹ 2,29,696</v>
+        <v>₹ 2,17,155</v>
       </c>
       <c r="D4" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E4" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F4" t="str">
-        <v>₹ 23,90,408</v>
+        <v>₹ 23,83,857</v>
       </c>
       <c r="G4" t="str">
-        <v>4.38%</v>
+        <v>4.65%</v>
       </c>
     </row>
     <row r="5">
@@ -499,22 +499,22 @@
         <v>2028</v>
       </c>
       <c r="B5" t="str">
-        <v>₹ 54,900</v>
+        <v>₹ 57,713</v>
       </c>
       <c r="C5" t="str">
-        <v>₹ 2,24,739</v>
+        <v>₹ 2,12,205</v>
       </c>
       <c r="D5" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E5" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F5" t="str">
-        <v>₹ 23,35,508</v>
+        <v>₹ 23,26,144</v>
       </c>
       <c r="G5" t="str">
-        <v>6.58%</v>
+        <v>6.95%</v>
       </c>
     </row>
     <row r="6">
@@ -522,22 +522,22 @@
         <v>2029</v>
       </c>
       <c r="B6" t="str">
-        <v>₹ 60,349</v>
+        <v>₹ 63,127</v>
       </c>
       <c r="C6" t="str">
-        <v>₹ 2,19,290</v>
+        <v>₹ 2,06,791</v>
       </c>
       <c r="D6" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E6" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F6" t="str">
-        <v>₹ 22,75,159</v>
+        <v>₹ 22,63,017</v>
       </c>
       <c r="G6" t="str">
-        <v>8.99%</v>
+        <v>9.48%</v>
       </c>
     </row>
     <row r="7">
@@ -545,22 +545,22 @@
         <v>2030</v>
       </c>
       <c r="B7" t="str">
-        <v>₹ 66,338</v>
+        <v>₹ 69,048</v>
       </c>
       <c r="C7" t="str">
-        <v>₹ 2,13,301</v>
+        <v>₹ 2,00,869</v>
       </c>
       <c r="D7" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E7" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F7" t="str">
-        <v>₹ 22,08,821</v>
+        <v>₹ 21,93,969</v>
       </c>
       <c r="G7" t="str">
-        <v>11.65%</v>
+        <v>12.24%</v>
       </c>
     </row>
     <row r="8">
@@ -568,22 +568,22 @@
         <v>2031</v>
       </c>
       <c r="B8" t="str">
-        <v>₹ 72,922</v>
+        <v>₹ 75,526</v>
       </c>
       <c r="C8" t="str">
-        <v>₹ 2,06,717</v>
+        <v>₹ 1,94,392</v>
       </c>
       <c r="D8" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E8" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F8" t="str">
-        <v>₹ 21,35,899</v>
+        <v>₹ 21,18,443</v>
       </c>
       <c r="G8" t="str">
-        <v>14.56%</v>
+        <v>15.26%</v>
       </c>
     </row>
     <row r="9">
@@ -591,22 +591,22 @@
         <v>2032</v>
       </c>
       <c r="B9" t="str">
-        <v>₹ 80,160</v>
+        <v>₹ 82,610</v>
       </c>
       <c r="C9" t="str">
-        <v>₹ 1,99,480</v>
+        <v>₹ 1,87,307</v>
       </c>
       <c r="D9" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E9" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F9" t="str">
-        <v>₹ 20,55,739</v>
+        <v>₹ 20,35,833</v>
       </c>
       <c r="G9" t="str">
-        <v>17.77%</v>
+        <v>18.57%</v>
       </c>
     </row>
     <row r="10">
@@ -614,22 +614,22 @@
         <v>2033</v>
       </c>
       <c r="B10" t="str">
-        <v>₹ 88,115</v>
+        <v>₹ 90,360</v>
       </c>
       <c r="C10" t="str">
-        <v>₹ 1,91,524</v>
+        <v>₹ 1,79,558</v>
       </c>
       <c r="D10" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E10" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F10" t="str">
-        <v>₹ 19,67,624</v>
+        <v>₹ 19,45,473</v>
       </c>
       <c r="G10" t="str">
-        <v>21.3%</v>
+        <v>22.18%</v>
       </c>
     </row>
     <row r="11">
@@ -637,22 +637,22 @@
         <v>2034</v>
       </c>
       <c r="B11" t="str">
-        <v>₹ 96,861</v>
+        <v>₹ 98,836</v>
       </c>
       <c r="C11" t="str">
-        <v>₹ 1,82,779</v>
+        <v>₹ 1,71,082</v>
       </c>
       <c r="D11" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E11" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F11" t="str">
-        <v>₹ 18,70,763</v>
+        <v>₹ 18,46,637</v>
       </c>
       <c r="G11" t="str">
-        <v>25.17%</v>
+        <v>26.13%</v>
       </c>
     </row>
     <row r="12">
@@ -660,22 +660,22 @@
         <v>2035</v>
       </c>
       <c r="B12" t="str">
-        <v>₹ 1,06,474</v>
+        <v>₹ 1,08,108</v>
       </c>
       <c r="C12" t="str">
-        <v>₹ 1,73,166</v>
+        <v>₹ 1,61,810</v>
       </c>
       <c r="D12" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E12" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F12" t="str">
-        <v>₹ 17,64,289</v>
+        <v>₹ 17,38,529</v>
       </c>
       <c r="G12" t="str">
-        <v>29.43%</v>
+        <v>30.46%</v>
       </c>
     </row>
     <row r="13">
@@ -683,22 +683,22 @@
         <v>2036</v>
       </c>
       <c r="B13" t="str">
-        <v>₹ 1,17,041</v>
+        <v>₹ 1,18,249</v>
       </c>
       <c r="C13" t="str">
-        <v>₹ 1,62,598</v>
+        <v>₹ 1,51,669</v>
       </c>
       <c r="D13" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E13" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F13" t="str">
-        <v>₹ 16,47,248</v>
+        <v>₹ 16,20,280</v>
       </c>
       <c r="G13" t="str">
-        <v>34.11%</v>
+        <v>35.19%</v>
       </c>
     </row>
     <row r="14">
@@ -706,22 +706,22 @@
         <v>2037</v>
       </c>
       <c r="B14" t="str">
-        <v>₹ 1,28,657</v>
+        <v>₹ 1,29,342</v>
       </c>
       <c r="C14" t="str">
-        <v>₹ 1,50,982</v>
+        <v>₹ 1,40,576</v>
       </c>
       <c r="D14" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E14" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F14" t="str">
-        <v>₹ 15,18,591</v>
+        <v>₹ 14,90,939</v>
       </c>
       <c r="G14" t="str">
-        <v>39.26%</v>
+        <v>40.36%</v>
       </c>
     </row>
     <row r="15">
@@ -729,22 +729,22 @@
         <v>2038</v>
       </c>
       <c r="B15" t="str">
-        <v>₹ 1,41,426</v>
+        <v>₹ 1,41,475</v>
       </c>
       <c r="C15" t="str">
-        <v>₹ 1,38,213</v>
+        <v>₹ 1,28,443</v>
       </c>
       <c r="D15" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E15" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F15" t="str">
-        <v>₹ 13,77,165</v>
+        <v>₹ 13,49,464</v>
       </c>
       <c r="G15" t="str">
-        <v>44.91%</v>
+        <v>46.02%</v>
       </c>
     </row>
     <row r="16">
@@ -752,22 +752,22 @@
         <v>2039</v>
       </c>
       <c r="B16" t="str">
-        <v>₹ 1,55,462</v>
+        <v>₹ 1,54,746</v>
       </c>
       <c r="C16" t="str">
-        <v>₹ 1,24,177</v>
+        <v>₹ 1,15,172</v>
       </c>
       <c r="D16" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E16" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F16" t="str">
-        <v>₹ 12,21,703</v>
+        <v>₹ 11,94,718</v>
       </c>
       <c r="G16" t="str">
-        <v>51.13%</v>
+        <v>52.21%</v>
       </c>
     </row>
     <row r="17">
@@ -775,22 +775,22 @@
         <v>2040</v>
       </c>
       <c r="B17" t="str">
-        <v>₹ 1,70,891</v>
+        <v>₹ 1,69,262</v>
       </c>
       <c r="C17" t="str">
-        <v>₹ 1,08,748</v>
+        <v>₹ 1,00,656</v>
       </c>
       <c r="D17" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E17" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F17" t="str">
-        <v>₹ 10,50,812</v>
+        <v>₹ 10,25,456</v>
       </c>
       <c r="G17" t="str">
-        <v>57.97%</v>
+        <v>58.98%</v>
       </c>
     </row>
     <row r="18">
@@ -798,22 +798,22 @@
         <v>2041</v>
       </c>
       <c r="B18" t="str">
-        <v>₹ 1,87,852</v>
+        <v>₹ 1,85,140</v>
       </c>
       <c r="C18" t="str">
-        <v>₹ 91,787</v>
+        <v>₹ 84,778</v>
       </c>
       <c r="D18" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E18" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F18" t="str">
-        <v>₹ 8,62,960</v>
+        <v>₹ 8,40,315</v>
       </c>
       <c r="G18" t="str">
-        <v>65.48%</v>
+        <v>66.39%</v>
       </c>
     </row>
     <row r="19">
@@ -821,22 +821,22 @@
         <v>2042</v>
       </c>
       <c r="B19" t="str">
-        <v>₹ 2,06,496</v>
+        <v>₹ 2,02,508</v>
       </c>
       <c r="C19" t="str">
-        <v>₹ 73,144</v>
+        <v>₹ 67,410</v>
       </c>
       <c r="D19" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E19" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F19" t="str">
-        <v>₹ 6,56,464</v>
+        <v>₹ 6,37,808</v>
       </c>
       <c r="G19" t="str">
-        <v>73.74%</v>
+        <v>74.49%</v>
       </c>
     </row>
     <row r="20">
@@ -844,22 +844,22 @@
         <v>2043</v>
       </c>
       <c r="B20" t="str">
-        <v>₹ 2,26,990</v>
+        <v>₹ 2,21,504</v>
       </c>
       <c r="C20" t="str">
-        <v>₹ 52,649</v>
+        <v>₹ 48,414</v>
       </c>
       <c r="D20" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E20" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F20" t="str">
-        <v>₹ 4,29,474</v>
+        <v>₹ 4,16,304</v>
       </c>
       <c r="G20" t="str">
-        <v>82.82%</v>
+        <v>83.35%</v>
       </c>
     </row>
     <row r="21">
@@ -867,22 +867,22 @@
         <v>2044</v>
       </c>
       <c r="B21" t="str">
-        <v>₹ 2,49,518</v>
+        <v>₹ 2,42,283</v>
       </c>
       <c r="C21" t="str">
-        <v>₹ 30,121</v>
+        <v>₹ 27,635</v>
       </c>
       <c r="D21" t="str">
         <v>₹ 37,500</v>
       </c>
       <c r="E21" t="str">
-        <v>₹ 3,17,139</v>
+        <v>₹ 3,07,418</v>
       </c>
       <c r="F21" t="str">
-        <v>₹ 1,79,956</v>
+        <v>₹ 1,74,021</v>
       </c>
       <c r="G21" t="str">
-        <v>92.8%</v>
+        <v>93.04%</v>
       </c>
     </row>
     <row r="22">
@@ -890,16 +890,16 @@
         <v>2045</v>
       </c>
       <c r="B22" t="str">
-        <v>₹ 1,79,956</v>
+        <v>₹ 1,74,021</v>
       </c>
       <c r="C22" t="str">
-        <v>₹ 6,470</v>
+        <v>₹ 5,924</v>
       </c>
       <c r="D22" t="str">
         <v>₹ 25,000</v>
       </c>
       <c r="E22" t="str">
-        <v>₹ 2,11,426</v>
+        <v>₹ 2,04,945</v>
       </c>
       <c r="F22" t="str">
         <v>₹ 0</v>

</xml_diff>